<commit_message>
Optimization Updates - Attribute Mapper
</commit_message>
<xml_diff>
--- a/FME_fmw_files/LOOKUP_TABLES/FormatAttributeMapper.xlsx
+++ b/FME_fmw_files/LOOKUP_TABLES/FormatAttributeMapper.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="54">
   <si>
     <t>original_value</t>
   </si>
@@ -503,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39:XFD39"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -709,39 +709,39 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="B25" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="B26" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="B27" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="B28" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B29" t="s">
         <v>13</v>
@@ -749,55 +749,55 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="B30" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B31" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="B32" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>12</v>
       </c>
       <c r="B33" t="s">
-        <v>45</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
       <c r="B34" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B35" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B36" t="s">
         <v>6</v>
@@ -805,17 +805,25 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B37" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>5</v>
+      </c>
+      <c r="B38" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>3</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>